<commit_message>
Sprint review protocol modified
</commit_message>
<xml_diff>
--- a/Org/Semester 2/Sprint_3.xlsx
+++ b/Org/Semester 2/Sprint_3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1548" windowWidth="38640" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-1545" windowWidth="38640" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -82,12 +82,6 @@
     <t>short description [opt]</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Mentor</t>
   </si>
   <si>
@@ -136,26 +130,26 @@
     <t>Implementierung von UI Elementen, um zwischen den jeweiligen Schnittebenen (transversal, sattigal, coronal) zu wechseln (Akzeptanzkriterium: User kann in VR mit Handtracking Buttons drücken, die zwischen den Schnittebenen wechseln)</t>
   </si>
   <si>
-    <t>UpdateFrame? Manuell (Name könnte in Unity anders sein)</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
     <t>Beim Import der Herzsegmente ist aufgefallen, dass der Speicherverbrauch um ein vielfaches Steigt und Unity zum Absturz bringt   -&gt; es wird eine Alternative im nächsten Sprint erarbeitet</t>
   </si>
   <si>
-    <t>Durch erhöhten Zeitaufwand durch Git Workflow konnte dieses Requirement nicht vollständig umgesetzt werden -&gt; wird in nächsten Sprint fortgesetzt</t>
-  </si>
-  <si>
     <t>Vorläufige Einfärbung des Herzens mithilfe der transfer function, um 2D Schnittebene testen zu können (Akzeptanzkriterium: Herz ist klar erkennbar und wird vom Rest der Voxel rundherum unterschieden)</t>
+  </si>
+  <si>
+    <t>Durch erhöhten Zeitaufwand (Git Workflow) konnte dieses Requirement nicht vollständig umgesetzt werden -&gt; wird in nächsten Sprint fortgesetzt</t>
+  </si>
+  <si>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,13 +196,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="6" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -437,25 +424,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -520,26 +517,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -869,187 +848,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="65.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.44140625" style="2"/>
-    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="65.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27">
         <v>3</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="27">
+      <c r="B5" s="16"/>
+      <c r="C5" s="29">
         <v>45776.708333333336</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="28">
+      <c r="B6" s="16"/>
+      <c r="C6" s="30">
         <v>16</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="21" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="21" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1057,13 +1036,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>11</v>
@@ -1075,251 +1054,184 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="32">
+    <row r="16" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>1</v>
       </c>
-      <c r="B16" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="36">
+      <c r="B16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="10">
         <v>3</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="10">
         <v>5</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="11">
         <f>D16-C16</f>
         <v>2</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="32">
+      <c r="F16" s="7"/>
+      <c r="G16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>2</v>
       </c>
-      <c r="B17" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="36">
+      <c r="B17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="10">
         <v>4</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="10">
         <v>3</v>
       </c>
-      <c r="E17" s="37">
-        <f t="shared" ref="E17:E25" si="0">D17-C17</f>
+      <c r="E17" s="11">
+        <f t="shared" ref="E17:E20" si="0">D17-C17</f>
         <v>-1</v>
       </c>
-      <c r="F17" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-    </row>
-    <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="32">
+      <c r="F17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>3</v>
       </c>
-      <c r="B18" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="36">
+      <c r="B18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="10">
         <v>20</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="10">
         <v>18</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="11">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F18" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="32">
+      <c r="F18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>4</v>
       </c>
-      <c r="B19" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="36">
+      <c r="B19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="10">
         <v>10</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D19" s="10">
         <v>18</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="11">
         <f>D19-C19</f>
         <v>8</v>
       </c>
-      <c r="F19" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="36"/>
-    </row>
-    <row r="20" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="32">
+      <c r="F19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>5</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="36">
+      <c r="B20" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="10">
         <v>7</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="10">
         <v>5</v>
       </c>
-      <c r="E20" s="37">
+      <c r="E20" s="11">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F20" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="36"/>
-    </row>
-    <row r="21" spans="1:8" ht="78" x14ac:dyDescent="0.3">
-      <c r="A21" s="32">
+      <c r="F20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>6</v>
       </c>
-      <c r="B21" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="36">
+      <c r="B21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="10">
         <v>15</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="10">
         <v>11</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="11">
         <f>D21-C21</f>
         <v>-4</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="8">
-        <v>7</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
-        <f>COUNT(A16:A25)</f>
-        <v>7</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <f>SUM(E16:E25)</f>
-        <v>1</v>
-      </c>
-      <c r="F26" s="6">
-        <f>COUNT(F16:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <f>COUNT(G16:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C27" s="2">
-        <f>SUM(C16:C22)</f>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="34">
+        <f>SUM(C16:C21)</f>
         <v>59</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D23" s="34">
         <f>SUM(D16:D21)</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
-        <v>22</v>
+      <c r="E23" s="34">
+        <f>SUM(E16:E21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1257,7 @@
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="C11:G11"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>